<commit_message>
Added performance improvments on Diary Index view Splited diary details into separate view
</commit_message>
<xml_diff>
--- a/Files/0000-1000/35/A35_RequestList.xlsx
+++ b/Files/0000-1000/35/A35_RequestList.xlsx
@@ -25,7 +25,7 @@
     <t>ОФИС гр. РУСЕ и ОФИС гр. СОФИЯ</t>
   </si>
   <si>
-    <t>ЗАЯВКА № A35 / Дата 25.06.2017</t>
+    <t>ЗАЯВКА № A35 / Дата 19.07.2017</t>
   </si>
   <si>
     <t>7.2 ФИЗИКОХИМИЧНО И ОРГАНОЛЕПТИЧНО ИЗПИТВАНЕ</t>
@@ -61,7 +61,7 @@
     <t xml:space="preserve">БДС 3485 т.3.5 </t>
   </si>
   <si>
-    <t>Срок за изпитване: 2 дни</t>
+    <t>Срок за изпитване: 3 дни</t>
   </si>
   <si>
     <t>Приел пробата......</t>

</xml_diff>